<commit_message>
Improved symbol handling and added all of the formulas from the math namespace.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -21,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -29,13 +29,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF484848"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,8 +74,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,37 +376,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:16">
       <c r="A1">
-        <v>1</v>
+        <f>SUM(1,2,3,4,5,6,7)</f>
+        <v>28</v>
       </c>
       <c r="B1">
+        <f>CODE("A")</f>
+        <v>65</v>
+      </c>
+      <c r="C1" t="str">
+        <f>IMCOS("1+i")</f>
+        <v>0.833730025131149-0.988897705762865i</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>IMSIN("3+4i")</f>
+        <v>3.85373803791938-27.0168132580039i</v>
+      </c>
+      <c r="E1">
+        <f>FACT(5)</f>
+        <v>120</v>
+      </c>
+      <c r="F1" s="2">
+        <f>FLOOR(0.234, 0.01)</f>
+        <v>0.23</v>
+      </c>
+      <c r="G1" s="3">
+        <f>LCM(24, 36)</f>
+        <v>72</v>
+      </c>
+      <c r="H1" s="2">
+        <f>MROUND(10, 3)</f>
+        <v>9</v>
+      </c>
+      <c r="I1" s="2">
+        <f>MROUND(1.3, 0.2)</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="J1" s="4">
+        <f>5/4</f>
+        <v>1.25</v>
+      </c>
+      <c r="K1" s="2">
+        <f ca="1">RAND()*100</f>
+        <v>6.0230292801129792</v>
+      </c>
+      <c r="L1" s="2">
+        <f>ROUNDDOWN(3.14159, 3)</f>
+        <v>3.141</v>
+      </c>
+      <c r="M1" s="2" t="str">
+        <f>ROMAN(499,0)</f>
+        <v>CDXCIX</v>
+      </c>
+      <c r="N1" s="2">
+        <f>SIN(PI())</f>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="O1" s="2">
+        <f>SQRTPI(1)</f>
+        <v>1.7724538509055159</v>
+      </c>
+      <c r="P1" s="2">
+        <f>SUMIF(A2:A5,4,B2:B5)</f>
+        <v>0.84270073517455524</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <f>AVERAGE(1,2,3,4,5,6,7)</f>
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>ERF(1)</f>
+        <v>0.84270073517455524</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IMDIV("-238+240i","10+24i")</f>
+        <v>5+12i</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>IMSQRT("1+i")</f>
+        <v>1.09868411346781+0.455089860562227i</v>
+      </c>
+      <c r="E2" s="2">
+        <f>FACT(1.9)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <f>GCD(5, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <f>MDETERM(D6:F8)</f>
+        <v>3402</v>
+      </c>
+      <c r="H2" s="2">
+        <f>MROUND(-10, -3)</f>
+        <v>-9</v>
+      </c>
+      <c r="I2" s="2">
+        <f>EVEN(1.5)</f>
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="J2" s="2">
+        <f>PRODUCT(A2:A4)</f>
+        <v>380.88657424836441</v>
+      </c>
+      <c r="K2" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>5</v>
+      </c>
+      <c r="L2" s="2">
+        <f>ROUNDDOWN(-3.14159, 1)</f>
+        <v>-3.1</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>ROMAN(499,1)</f>
+        <v>LDVLIV</v>
+      </c>
+      <c r="N2" s="2">
+        <f>SIN(PI()/2)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <f>SQRTPI(2)</f>
+        <v>2.5066282746310002</v>
+      </c>
+      <c r="P2" s="2">
+        <f>SUMIF(A2:A7,"Fruits",C2:C7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <f>CODE("asdf")</f>
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <f>ERFC(1)</f>
+        <v>0.15729926482544476</v>
+      </c>
+      <c r="C3" t="str">
+        <f>IMEXP("1+i")</f>
+        <v>1.46869393991589+2.28735528717884i</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>IMSUB("13+4i","5+3i")</f>
+        <v>8+i</v>
+      </c>
+      <c r="E3" s="2">
+        <f>FACT(0)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <f>GCD(24, 36)</f>
+        <v>12</v>
+      </c>
+      <c r="G3" s="2">
+        <f>MDETERM({3,6,1;1,1,0;3,10,2})</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="H3" s="2">
+        <f>MULTINOMIAL(2, 3, 4)</f>
+        <v>1259.9999999999991</v>
+      </c>
+      <c r="I3" s="2">
+        <f>EVEN(3)</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="2">
+        <f>PRODUCT(A2:A4, 2)</f>
+        <v>761.77314849672882</v>
+      </c>
+      <c r="K3" s="2">
+        <f ca="1">RANDBETWEEN(-1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <f>ROUNDDOWN(31415.92654, -2)</f>
+        <v>31400</v>
+      </c>
+      <c r="M3" s="2" t="str">
+        <f>ROMAN(499,2)</f>
+        <v>XDIX</v>
+      </c>
+      <c r="N3" s="2">
+        <f>SIN(30*PI()/180)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="O3" s="2">
+        <f>SUM(3, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="P3" s="2">
+        <f>SUMPRODUCT(A2:A4, E2:E4)</f>
+        <v>101.98166642847517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <f>BESSELI(1.5,1)</f>
+        <v>0.98166642847516605</v>
+      </c>
+      <c r="B4">
+        <f>DELTA(100,100)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IMLN("1+i")</f>
+        <v>0.346573590279973+0.785398163397448i</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>IMSUM("3+4i","5-3i")</f>
+        <v>8+i</v>
+      </c>
+      <c r="E4" s="2">
+        <f>FACT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <f>GCD(7, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f>MDETERM({3,6;1,1})</f>
+        <v>-3</v>
+      </c>
+      <c r="H4" s="2">
+        <f>ODD(1.5)</f>
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="I4" s="2">
+        <f>EVEN(2)</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <f>A2*A3*A4</f>
+        <v>380.88657424836441</v>
+      </c>
+      <c r="K4" s="2">
+        <f>ROUND(2.15, 1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L4" s="2">
+        <f>ROUNDUP(3.2,0)</f>
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="M4" s="2" t="str">
+        <f>ROMAN(499,3)</f>
+        <v>VDIV</v>
+      </c>
+      <c r="N4" s="2">
+        <f>SIN(RADIANS(30))</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="O4" s="2">
+        <f>SUM("5", 15, TRUE)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <f>BESSELK(1.5,1)</f>
+        <v>0.27738780363225868</v>
+      </c>
+      <c r="B5">
+        <f>GESTEP(5,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>IMLOG10("1+i")</f>
+        <v>0.150514997831991+0.34109408846046i</v>
+      </c>
+      <c r="D5" s="2">
+        <f>CEILING(0.234, 0.01)</f>
+        <v>0.24</v>
+      </c>
+      <c r="E5" s="2">
+        <f>FACTDOUBLE(6)</f>
+        <v>48</v>
+      </c>
+      <c r="F5" s="2">
+        <f>GCD(5, 0)</f>
         <v>5</v>
       </c>
-      <c r="F1">
-        <f>SUM(A1:E1)</f>
-        <v>15</v>
-      </c>
+      <c r="G5" s="2">
+        <f>MINVERSE({3,6;1,1})</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="H5" s="2">
+        <f>ODD(3)</f>
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <f>EVEN(-1)</f>
+        <v>-2</v>
+      </c>
+      <c r="J5" s="2">
+        <f>QUOTIENT(5, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <f>ROUND(2.149, 1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="L5" s="2">
+        <f>ROUNDUP(76.9,0)</f>
+        <v>77</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f>ROMAN(499,4)</f>
+        <v>ID</v>
+      </c>
+      <c r="N5" s="2">
+        <f>SINH(1)</f>
+        <v>1.1752011936438014</v>
+      </c>
+      <c r="O5" s="2">
+        <f>SUM(A2:A4)</f>
+        <v>101.98166642847517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <f>BIN2DEC(10111)</f>
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <f>IMABS("5+12i")</f>
+        <v>13</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IMLOG2("1+i")</f>
+        <v>0.500000000038482+1.13309003554401i</v>
+      </c>
+      <c r="D6" s="2">
+        <f>COMBIN(8,2)</f>
+        <v>28</v>
+      </c>
+      <c r="E6" s="2">
+        <f>FACTDOUBLE(7)</f>
+        <v>105</v>
+      </c>
+      <c r="F6" s="2">
+        <f>INT(8.9)</f>
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <f>MINVERSE({3,6,1;1,1,0;3,10,2})</f>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="H6" s="2">
+        <f>ODD(2)</f>
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="J6" s="2">
+        <f>QUOTIENT(4.5, 3.1)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <f>ROUND(-1.475, 2)</f>
+        <v>-1.48</v>
+      </c>
+      <c r="L6" s="2">
+        <f>ROUNDUP(3.14159, 3)</f>
+        <v>3.1419999999999999</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f>ROMAN(2013,0)</f>
+        <v>MMXIII</v>
+      </c>
+      <c r="N6" s="2">
+        <f>SINH(-1)</f>
+        <v>-1.1752011936438014</v>
+      </c>
+      <c r="O6" s="2">
+        <f>SUM(A2:A4, 15)</f>
+        <v>116.98166642847517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="str">
+        <f>DEC2BIN(23)</f>
+        <v>10111</v>
+      </c>
+      <c r="B7">
+        <f>IMAGINARY("0-j")</f>
+        <v>-1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IMPOWER("2+3i", 3)</f>
+        <v>-46+9.00000000000001i</v>
+      </c>
+      <c r="D7">
+        <f>CODE("A1:E3")</f>
+        <v>65</v>
+      </c>
+      <c r="E7" s="2">
+        <f>FLOOR(-2.5, -2)</f>
+        <v>-2</v>
+      </c>
+      <c r="F7" s="2">
+        <f>INT(-8.9)</f>
+        <v>-9</v>
+      </c>
+      <c r="G7">
+        <f>MMULT({3,6,1;1,1,0;3,10,2},{3,6,1;1,1,0;3,10,2})</f>
+        <v>18</v>
+      </c>
+      <c r="H7" s="2">
+        <f>ODD(-1)</f>
+        <v>-1</v>
+      </c>
+      <c r="I7" s="2">
+        <f>POWER(5,2)</f>
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <f>QUOTIENT(-10, 3)</f>
+        <v>-3</v>
+      </c>
+      <c r="K7" s="2">
+        <f>ROUND(21.5, -1)</f>
+        <v>20</v>
+      </c>
+      <c r="L7" s="2">
+        <f>ROUNDUP(-3.14159, 1)</f>
+        <v>-3.2</v>
+      </c>
+      <c r="M7" s="2">
+        <f>SIGN(10)</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <f>2.868*SINH(0.0342*1.03)</f>
+        <v>0.10104906311828733</v>
+      </c>
+      <c r="O7" s="2">
+        <f>SUM(A5,A6, 2)</f>
+        <v>25.277387803632259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="str">
+        <f>COMPLEX(1,1)</f>
+        <v>1+i</v>
+      </c>
+      <c r="B8">
+        <f>IMARGUMENT("3+4i")</f>
+        <v>0.92729521800161219</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IMPRODUCT("1+2i",30)</f>
+        <v>30+60i</v>
+      </c>
+      <c r="D8" s="2">
+        <f>EVEN(-1)</f>
+        <v>-2</v>
+      </c>
+      <c r="E8" s="2">
+        <f>FLOOR(2.5, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <f>A2-INT(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>MMULT({2,1;1,2},{3,4;4,3})</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <f>ODD(-2)</f>
+        <v>-3</v>
+      </c>
+      <c r="I8" s="2">
+        <f>POWER(98.6,3.2)</f>
+        <v>2401077.2220695755</v>
+      </c>
+      <c r="J8" s="2">
+        <f>RADIANS(270)</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="K8" s="2">
+        <f>ROUNDDOWN(3.2, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="L8" s="2">
+        <f>ROUNDUP(31415.92654, -2)</f>
+        <v>31500</v>
+      </c>
+      <c r="M8" s="2">
+        <f>SIGN(4-4)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <f>SQRT(16)</f>
+        <v>4</v>
+      </c>
+      <c r="O8" s="2">
+        <f>SUMIF(A2:A5,"&gt;1",B2:B5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <f>CODE("A1:E3")</f>
+        <v>65</v>
+      </c>
+      <c r="B9" t="str">
+        <f>IMCONJUGATE("3+4i")</f>
+        <v>3-4i</v>
+      </c>
+      <c r="C9" s="2">
+        <f>IMREAL("6-9i")</f>
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <f>EXP(2)</f>
+        <v>7.3890560989306504</v>
+      </c>
+      <c r="E9" s="2">
+        <f>FLOOR(1.5, 0.1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="2">
+        <f>LCM(5, 2)</f>
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <f>MOD(-3, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <f>MROUND(-10, -3)</f>
+        <v>-9</v>
+      </c>
+      <c r="I9" s="2">
+        <f>POWER(4,5/4)</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="J9" s="2">
+        <f ca="1">RAND()</f>
+        <v>0.28082032582331529</v>
+      </c>
+      <c r="K9" s="2">
+        <f>ROUNDDOWN(76.9,0)</f>
+        <v>76</v>
+      </c>
+      <c r="L9" s="2">
+        <f>SERIESSUM(2,0,2,{1,2,3,4,5})</f>
+        <v>1593</v>
+      </c>
+      <c r="M9" s="2">
+        <f>SIGN(-0.00001)</f>
+        <v>-1</v>
+      </c>
+      <c r="N9" s="2">
+        <f>SQRT(ABS(A2))</f>
+        <v>2</v>
+      </c>
+      <c r="O9" s="2">
+        <f>SUMIF(A2:A5,"&gt;1")</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>